<commit_message>
chenges in xls file
</commit_message>
<xml_diff>
--- a/TestNGFW/src/test/java/com_xls/Excelsheet1.xlsx
+++ b/TestNGFW/src/test/java/com_xls/Excelsheet1.xlsx
@@ -1,34 +1,47 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14100" windowHeight="5520"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>username</t>
   </si>
   <si>
     <t>password</t>
   </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>PASS123</t>
+  </si>
+  <si>
+    <t>XYZ</t>
+  </si>
+  <si>
+    <t>PASS456</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -65,6 +78,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -143,6 +161,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -177,6 +196,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -352,21 +372,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -375,24 +411,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>